<commit_message>
Remove conditional formatter from demo
Change-Id: I8bf2e2fdc52927457f4c41c09ea01e6b1ad4a22a
</commit_message>
<xml_diff>
--- a/src/main/resources/testsheets/Named Ranges Chart.xlsx
+++ b/src/main/resources/testsheets/Named Ranges Chart.xlsx
@@ -316,7 +316,14 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
@@ -328,14 +335,7 @@
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -513,11 +513,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="37"/>
-        <c:axId val="33073648"/>
-        <c:axId val="53969504"/>
+        <c:axId val="-685886656"/>
+        <c:axId val="-685857184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="33073648"/>
+        <c:axId val="-685886656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +549,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53969504"/>
+        <c:crossAx val="-685857184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -557,7 +557,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53969504"/>
+        <c:axId val="-685857184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -588,7 +588,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33073648"/>
+        <c:crossAx val="-685886656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="500.0"/>
@@ -766,7 +766,7 @@
   <autoFilter ref="B4:C7"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Amount" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="Amount" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="Simple Monthly Budget" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -782,7 +782,7 @@
   <autoFilter ref="B10:C23"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Amount" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="2" name="Amount" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Simple Monthly Budget" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1071,7 +1071,7 @@
   <dimension ref="B1:H23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="G9" sqref="G9:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1299,11 +1299,6 @@
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G9:H9"/>
   </mergeCells>
-  <conditionalFormatting sqref="G9:H9">
-    <cfRule type="expression" dxfId="4" priority="1">
-      <formula>$G$9&lt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix 1.3 demo file with named ranges in chart and formatting rule
Change-Id: Ia0218dcc4db4214586cb4357b7c099ffd1d2d2e6
</commit_message>
<xml_diff>
--- a/src/main/resources/testsheets/Named Ranges Chart.xlsx
+++ b/src/main/resources/testsheets/Named Ranges Chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guille/Projects/spreadsheet-demo/src/main/resources/testsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guille/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -314,7 +314,27 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -360,8 +380,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Simple Monthly Budget" pivot="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="wholeTable" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -513,11 +533,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="37"/>
-        <c:axId val="-685886656"/>
-        <c:axId val="-685857184"/>
+        <c:axId val="-348915920"/>
+        <c:axId val="-350485840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-685886656"/>
+        <c:axId val="-348915920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +569,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-685857184"/>
+        <c:crossAx val="-350485840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -557,7 +577,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-685857184"/>
+        <c:axId val="-350485840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -588,7 +608,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-685886656"/>
+        <c:crossAx val="-348915920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:minorUnit val="500.0"/>
@@ -766,7 +786,7 @@
   <autoFilter ref="B4:C7"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Amount" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="2" name="Amount" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="Simple Monthly Budget" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -782,7 +802,7 @@
   <autoFilter ref="B10:C23"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Item" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Amount" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="2" name="Amount" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="Simple Monthly Budget" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1299,6 +1319,11 @@
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G9:H9"/>
   </mergeCells>
+  <conditionalFormatting sqref="G9:H9">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>